<commit_message>
4.29 Advance the story line
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Q1C1.xlsx
+++ b/Assets/StreamingAssets/Q1C1.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renqi/TextAdvancedGame/Assets/StreamingAssets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B3C141-6833-C74D-8967-F4C45C0E02B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94218357-4AFD-744C-908E-CF5069DB4335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-280" yWindow="500" windowWidth="28100" windowHeight="15940" xr2:uid="{68C9ECD6-F2C7-A34A-8665-FFA8663C762C}"/>
+    <workbookView xWindow="700" yWindow="500" windowWidth="28100" windowHeight="15940" xr2:uid="{68C9ECD6-F2C7-A34A-8665-FFA8663C762C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -106,10 +106,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>End of story</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Waterfall</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -150,6 +146,30 @@
   </si>
   <si>
     <t>Bridge-Connect</t>
+  </si>
+  <si>
+    <t>LastBGImage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LastBGM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LastX1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LastX2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Goto</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StoryScript2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -536,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EEC272-F350-D34D-A243-3179172F76FB}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -549,9 +569,11 @@
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="19.5" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="13" max="13" width="17.83203125" customWidth="1"/>
+    <col min="14" max="14" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17">
+    <row r="1" spans="1:16" ht="17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -588,39 +610,51 @@
       <c r="L1" t="s">
         <v>13</v>
       </c>
+      <c r="M1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="17">
+    <row r="2" spans="1:16" ht="17">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="51">
+    <row r="3" spans="1:16" ht="51">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
@@ -629,57 +663,124 @@
         <v>-500</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="M3" t="str">
+        <f>IF(E2&lt;&gt;"",E2,M2)</f>
+        <v>Bridge-Connect</v>
+      </c>
+      <c r="N3" t="str">
+        <f>IF(F2&lt;&gt;"",F2,N2)</f>
+        <v>Waterfall</v>
+      </c>
+      <c r="O3">
+        <f>IF(H2&lt;&gt;"",H2,O2)</f>
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <f>IF(K2&lt;&gt;"",K2,P2)</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="34">
+    <row r="4" spans="1:16" ht="34">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" ref="M4:M6" si="0">IF(E3&lt;&gt;"",E3,M3)</f>
+        <v>Bridge-Connect</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" ref="N4:N6" si="1">IF(F3&lt;&gt;"",F3,N3)</f>
+        <v>Waterfall</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O6" si="2">IF(H3&lt;&gt;"",H3,O3)</f>
+        <v>-500</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P6" si="3">IF(K3&lt;&gt;"",K3,P3)</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="34">
+    <row r="5" spans="1:16" ht="34">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" t="s">
-        <v>26</v>
+      <c r="M5" t="str">
+        <f t="shared" si="0"/>
+        <v>Bridge-Connect</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="1"/>
+        <v>Waterfall</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="2"/>
+        <v>-500</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="17">
+    <row r="6" spans="1:16" ht="17">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="0"/>
+        <v>Bridge-Connect</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="1"/>
+        <v>Waterfall</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="2"/>
+        <v>-500</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:16" ht="17">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>32</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
5.17 Add Character Assets
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Q1C1.xlsx
+++ b/Assets/StreamingAssets/Q1C1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renqi/TextAdvancedGame/Assets/StreamingAssets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94218357-4AFD-744C-908E-CF5069DB4335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13579CA6-5154-DD4D-9CB7-11E000D5A0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="500" windowWidth="28100" windowHeight="15940" xr2:uid="{68C9ECD6-F2C7-A34A-8665-FFA8663C762C}"/>
   </bookViews>
@@ -106,10 +106,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Waterfall</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>You're right.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -169,6 +165,10 @@
   </si>
   <si>
     <t>StoryScript2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Happy</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -559,7 +559,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -611,16 +611,16 @@
         <v>13</v>
       </c>
       <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
         <v>28</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>29</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>30</v>
-      </c>
-      <c r="P1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="17">
@@ -628,19 +628,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="51">
@@ -648,13 +648,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
@@ -663,7 +663,7 @@
         <v>-500</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M3" t="str">
         <f>IF(E2&lt;&gt;"",E2,M2)</f>
@@ -671,7 +671,7 @@
       </c>
       <c r="N3" t="str">
         <f>IF(F2&lt;&gt;"",F2,N2)</f>
-        <v>Waterfall</v>
+        <v>Happy</v>
       </c>
       <c r="O3">
         <f>IF(H2&lt;&gt;"",H2,O2)</f>
@@ -687,13 +687,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M4" t="str">
         <f t="shared" ref="M4:M6" si="0">IF(E3&lt;&gt;"",E3,M3)</f>
@@ -701,7 +701,7 @@
       </c>
       <c r="N4" t="str">
         <f t="shared" ref="N4:N6" si="1">IF(F3&lt;&gt;"",F3,N3)</f>
-        <v>Waterfall</v>
+        <v>Happy</v>
       </c>
       <c r="O4">
         <f t="shared" ref="O4:O6" si="2">IF(H3&lt;&gt;"",H3,O3)</f>
@@ -714,19 +714,19 @@
     </row>
     <row r="5" spans="1:16" ht="34">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
         <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" si="0"/>
@@ -734,7 +734,7 @@
       </c>
       <c r="N5" t="str">
         <f t="shared" si="1"/>
-        <v>Waterfall</v>
+        <v>Happy</v>
       </c>
       <c r="O5">
         <f t="shared" si="2"/>
@@ -750,13 +750,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="0"/>
@@ -764,7 +764,7 @@
       </c>
       <c r="N6" t="str">
         <f t="shared" si="1"/>
-        <v>Waterfall</v>
+        <v>Happy</v>
       </c>
       <c r="O6">
         <f t="shared" si="2"/>
@@ -777,10 +777,10 @@
     </row>
     <row r="7" spans="1:16" ht="17">
       <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
5.17 Add History Image & Action
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Q1C1.xlsx
+++ b/Assets/StreamingAssets/Q1C1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renqi/TextAdvancedGame/Assets/StreamingAssets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13579CA6-5154-DD4D-9CB7-11E000D5A0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB151DE-2F48-5F4C-8BF8-918A004AF05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="500" windowWidth="28100" windowHeight="15940" xr2:uid="{68C9ECD6-F2C7-A34A-8665-FFA8663C762C}"/>
+    <workbookView xWindow="700" yWindow="500" windowWidth="28100" windowHeight="15820" xr2:uid="{68C9ECD6-F2C7-A34A-8665-FFA8663C762C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -169,6 +169,14 @@
   </si>
   <si>
     <t>Happy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>History</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HistoryAction</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -556,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EEC272-F350-D34D-A243-3179172F76FB}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -571,9 +579,10 @@
     <col min="5" max="5" width="22.33203125" customWidth="1"/>
     <col min="13" max="13" width="17.83203125" customWidth="1"/>
     <col min="14" max="14" width="15.83203125" customWidth="1"/>
+    <col min="18" max="18" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17">
+    <row r="1" spans="1:18" ht="17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -622,8 +631,14 @@
       <c r="P1" t="s">
         <v>30</v>
       </c>
+      <c r="Q1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" ht="17">
+    <row r="2" spans="1:18" ht="17">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -643,7 +658,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="51">
+    <row r="3" spans="1:18" ht="51">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -682,7 +697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="34">
+    <row r="4" spans="1:18" ht="34">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -712,7 +727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="34">
+    <row r="5" spans="1:18" ht="34">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -745,7 +760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="17">
+    <row r="6" spans="1:18" ht="17">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -775,7 +790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="17">
+    <row r="7" spans="1:18" ht="17">
       <c r="A7" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
5.31 Add SoundEffect & Optimise Save Function
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Q1C1.xlsx
+++ b/Assets/StreamingAssets/Q1C1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renqi/TextAdvancedGame/Assets/StreamingAssets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB151DE-2F48-5F4C-8BF8-918A004AF05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500A552D-154D-6B42-8543-EBD38ECA20F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="500" windowWidth="28100" windowHeight="15820" xr2:uid="{68C9ECD6-F2C7-A34A-8665-FFA8663C762C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -177,6 +177,14 @@
   </si>
   <si>
     <t>HistoryAction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SoundEffect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEAction</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -564,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EEC272-F350-D34D-A243-3179172F76FB}">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -582,7 +590,7 @@
     <col min="18" max="18" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17">
+    <row r="1" spans="1:20" ht="17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -637,8 +645,14 @@
       <c r="R1" t="s">
         <v>35</v>
       </c>
+      <c r="S1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" ht="17">
+    <row r="2" spans="1:20" ht="17">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -658,7 +672,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="51">
+    <row r="3" spans="1:20" ht="51">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -697,7 +711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="34">
+    <row r="4" spans="1:20" ht="34">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -727,7 +741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="34">
+    <row r="5" spans="1:20" ht="34">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -760,7 +774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="17">
+    <row r="6" spans="1:20" ht="17">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -790,7 +804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="17">
+    <row r="7" spans="1:20" ht="17">
       <c r="A7" t="s">
         <v>31</v>
       </c>

</xml_diff>